<commit_message>
Add group name to events excel report
</commit_message>
<xml_diff>
--- a/templates/export/events.xlsx
+++ b/templates/export/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sainathavadhuta/Documents/code/traccar/templates/export/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E82D36CA-D150-0C47-9D90-1B8846ACFEA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{395FF253-27C4-5F40-A45B-EEAA82F90C35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="18360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
             <family val="2"/>
             <charset val="204"/>
           </rPr>
-          <t>jx:area(lastCell="G7")</t>
+          <t>jx:area(lastCell="H7")</t>
         </r>
       </text>
     </comment>
@@ -54,7 +54,7 @@
             <family val="2"/>
             <charset val="204"/>
           </rPr>
-          <t>jx:each(items="devices", var="device", lastCell="G7" multisheet="sheetNames")</t>
+          <t>jx:each(items="devices", var="device", lastCell="H7" multisheet="sheetNames")</t>
         </r>
       </text>
     </comment>
@@ -68,7 +68,7 @@
             <family val="2"/>
             <charset val="204"/>
           </rPr>
-          <t>jx:each(items="device.objects", var="event", lastCell="G7")</t>
+          <t>jx:each(items="device.objects", var="event", lastCell="H7")</t>
         </r>
       </text>
     </comment>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Report type:</t>
   </si>
@@ -131,6 +131,12 @@
   </si>
   <si>
     <t>${event.deviceName}</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>${event.groupName}</t>
   </si>
 </sst>
 </file>
@@ -251,48 +257,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="15"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="15"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="15"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1027,113 +1029,120 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="29.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="37.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="38.5" style="1" customWidth="1"/>
-    <col min="5" max="6" width="55.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" customWidth="1"/>
+    <col min="3" max="3" width="37.33203125" customWidth="1"/>
+    <col min="4" max="4" width="38.5" customWidth="1"/>
+    <col min="5" max="6" width="55.5" customWidth="1"/>
     <col min="7" max="7" width="20.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4"/>
+    <row r="1" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="2"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="8"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="7"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
+    <row r="6" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="10" t="s">
         <v>16</v>
       </c>
+      <c r="H6" s="10" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
+    <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="14" t="s">
         <v>17</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>